<commit_message>
specialisatie ipv afgeleid van bij TGs
</commit_message>
<xml_diff>
--- a/standaarden/Standaarden.xlsx
+++ b/standaarden/Standaarden.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITREPO\bp4mc2-dcat\standaarden\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcobrattinga/GITREPO/bp4mc2-dcat/standaarden/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B708E8-CADA-EE44-AB0C-7EC296E9CA65}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="18195" windowHeight="7485" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="20720" windowHeight="14360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -390,7 +391,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,8 +457,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standaard 2" xfId="1"/>
-    <cellStyle name="Standaard 3" xfId="2"/>
+    <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Standaard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -475,7 +476,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -513,7 +514,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -548,6 +549,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -583,9 +601,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -758,23 +793,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -791,7 +826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -802,7 +837,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -816,7 +851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -830,7 +865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -844,7 +879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -858,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -872,7 +907,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -886,7 +921,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -900,7 +935,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -914,7 +949,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -925,7 +960,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -936,7 +971,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -947,7 +982,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -965,23 +1000,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1039,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -1021,7 +1056,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
@@ -1038,7 +1073,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1055,7 +1090,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1107,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1089,7 +1124,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -1103,7 +1138,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -1117,7 +1152,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>36</v>
       </c>
@@ -1131,7 +1166,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1180,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1165,28 +1200,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1218,7 +1253,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1241,7 +1276,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1267,7 +1302,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1293,7 +1328,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -1322,7 +1357,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1342,7 +1377,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1365,7 +1400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -1384,11 +1419,11 @@
       <c r="G8" t="s">
         <v>66</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -1410,11 +1445,11 @@
       <c r="H9" t="s">
         <v>60</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -1440,7 +1475,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1469,7 +1504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -1492,7 +1527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -1518,7 +1553,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1541,7 +1576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -1564,7 +1599,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -1584,7 +1619,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>86</v>
       </c>

</xml_diff>